<commit_message>
Added more user stories.
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Documents\Team 9 Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Ignore\Team9\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -48,6 +48,27 @@
   </si>
   <si>
     <t>As a user, I want to view the data in real-time</t>
+  </si>
+  <si>
+    <t>As a user, I want the data to be displayed in a dynamic, easily readable format.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to see both current and historic data.</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to easily navigate the interface.</t>
+  </si>
+  <si>
+    <t>As a developer, I want to be able to easily implement the API.</t>
+  </si>
+  <si>
+    <t>As a developer, I want the API to be well documented and understandable.</t>
+  </si>
+  <si>
+    <t>As a business, we want the product to have a unique selling point.</t>
+  </si>
+  <si>
+    <t>As a user, I want the different data to be easily distinguishable.</t>
   </si>
 </sst>
 </file>
@@ -405,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,10 +454,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -447,7 +468,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -455,24 +476,107 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
         <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>